<commit_message>
uploaded MLP model results
</commit_message>
<xml_diff>
--- a/net18/validation_data/Scenario1.xlsx
+++ b/net18/validation_data/Scenario1.xlsx
@@ -465,7 +465,7 @@
         <v>1.009610254607564</v>
       </c>
       <c r="G2" t="n">
-        <v>1.007160425186157</v>
+        <v>1.01953387260437</v>
       </c>
     </row>
     <row r="3">
@@ -492,7 +492,7 @@
         <v>1.016476486950764</v>
       </c>
       <c r="G3" t="n">
-        <v>1.017457842826843</v>
+        <v>1.02214777469635</v>
       </c>
     </row>
     <row r="4">
@@ -519,7 +519,7 @@
         <v>1.023316741954023</v>
       </c>
       <c r="G4" t="n">
-        <v>1.016798377037048</v>
+        <v>1.019710302352905</v>
       </c>
     </row>
     <row r="5">
@@ -546,7 +546,7 @@
         <v>1.023364330000336</v>
       </c>
       <c r="G5" t="n">
-        <v>1.007441759109497</v>
+        <v>1.026696681976318</v>
       </c>
     </row>
     <row r="6">
@@ -573,7 +573,7 @@
         <v>1.026025634011175</v>
       </c>
       <c r="G6" t="n">
-        <v>1.020978569984436</v>
+        <v>1.029133081436157</v>
       </c>
     </row>
     <row r="7">
@@ -600,7 +600,7 @@
         <v>1.026199926318352</v>
       </c>
       <c r="G7" t="n">
-        <v>1.014643669128418</v>
+        <v>1.02318811416626</v>
       </c>
     </row>
     <row r="8">
@@ -627,7 +627,7 @@
         <v>1.026453977738033</v>
       </c>
       <c r="G8" t="n">
-        <v>1.01308274269104</v>
+        <v>1.022620916366577</v>
       </c>
     </row>
     <row r="9">
@@ -654,7 +654,7 @@
         <v>1.026757375641291</v>
       </c>
       <c r="G9" t="n">
-        <v>1.013322710990906</v>
+        <v>1.02508008480072</v>
       </c>
     </row>
     <row r="10">
@@ -681,7 +681,7 @@
         <v>1.027484927913494</v>
       </c>
       <c r="G10" t="n">
-        <v>1.009721755981445</v>
+        <v>1.023085594177246</v>
       </c>
     </row>
     <row r="11">
@@ -708,7 +708,7 @@
         <v>1.02752103198984</v>
       </c>
       <c r="G11" t="n">
-        <v>1.016029715538025</v>
+        <v>1.02351188659668</v>
       </c>
     </row>
     <row r="12">
@@ -735,7 +735,7 @@
         <v>1.028363406436452</v>
       </c>
       <c r="G12" t="n">
-        <v>1.018782734870911</v>
+        <v>1.022902965545654</v>
       </c>
     </row>
     <row r="13">
@@ -762,7 +762,7 @@
         <v>1.0283301717721</v>
       </c>
       <c r="G13" t="n">
-        <v>1.011973738670349</v>
+        <v>1.019252777099609</v>
       </c>
     </row>
     <row r="14">
@@ -789,7 +789,7 @@
         <v>1.044251762033414</v>
       </c>
       <c r="G14" t="n">
-        <v>1.023491978645325</v>
+        <v>1.023057222366333</v>
       </c>
     </row>
     <row r="15">
@@ -816,7 +816,7 @@
         <v>1.04492271942274</v>
       </c>
       <c r="G15" t="n">
-        <v>1.016759157180786</v>
+        <v>1.027686476707458</v>
       </c>
     </row>
     <row r="16">
@@ -843,7 +843,7 @@
         <v>1.023190609422364</v>
       </c>
       <c r="G16" t="n">
-        <v>1.017158508300781</v>
+        <v>1.020583033561707</v>
       </c>
     </row>
     <row r="17">
@@ -870,7 +870,7 @@
         <v>1.023114485772568</v>
       </c>
       <c r="G17" t="n">
-        <v>1.013294100761414</v>
+        <v>1.022072911262512</v>
       </c>
     </row>
     <row r="18">
@@ -897,7 +897,7 @@
         <v>1.023072713401121</v>
       </c>
       <c r="G18" t="n">
-        <v>1.018951177597046</v>
+        <v>1.022224307060242</v>
       </c>
     </row>
     <row r="19">
@@ -924,7 +924,7 @@
         <v>1.023039265031769</v>
       </c>
       <c r="G19" t="n">
-        <v>1.015292644500732</v>
+        <v>1.026463747024536</v>
       </c>
     </row>
     <row r="20">
@@ -1659,7 +1659,7 @@
         <v>1.011403376800376</v>
       </c>
       <c r="G2" t="n">
-        <v>1.008413553237915</v>
+        <v>1.021594643592834</v>
       </c>
     </row>
     <row r="3">
@@ -1686,7 +1686,7 @@
         <v>1.018252058687226</v>
       </c>
       <c r="G3" t="n">
-        <v>1.018411874771118</v>
+        <v>1.023833155632019</v>
       </c>
     </row>
     <row r="4">
@@ -1713,7 +1713,7 @@
         <v>1.025101075990773</v>
       </c>
       <c r="G4" t="n">
-        <v>1.018298029899597</v>
+        <v>1.021430492401123</v>
       </c>
     </row>
     <row r="5">
@@ -1740,7 +1740,7 @@
         <v>1.02514865054941</v>
       </c>
       <c r="G5" t="n">
-        <v>1.008511066436768</v>
+        <v>1.028966069221497</v>
       </c>
     </row>
     <row r="6">
@@ -1767,7 +1767,7 @@
         <v>1.027809866721116</v>
       </c>
       <c r="G6" t="n">
-        <v>1.022449731826782</v>
+        <v>1.030413389205933</v>
       </c>
     </row>
     <row r="7">
@@ -1794,7 +1794,7 @@
         <v>1.027984181911415</v>
       </c>
       <c r="G7" t="n">
-        <v>1.016225457191467</v>
+        <v>1.024636745452881</v>
       </c>
     </row>
     <row r="8">
@@ -1821,7 +1821,7 @@
         <v>1.028237317852879</v>
       </c>
       <c r="G8" t="n">
-        <v>1.01434338092804</v>
+        <v>1.024176955223083</v>
       </c>
     </row>
     <row r="9">
@@ -1848,7 +1848,7 @@
         <v>1.028543542261516</v>
       </c>
       <c r="G9" t="n">
-        <v>1.015103340148926</v>
+        <v>1.026232361793518</v>
       </c>
     </row>
     <row r="10">
@@ -1875,7 +1875,7 @@
         <v>1.029273545776454</v>
       </c>
       <c r="G10" t="n">
-        <v>1.011108040809631</v>
+        <v>1.024853467941284</v>
       </c>
     </row>
     <row r="11">
@@ -1902,7 +1902,7 @@
         <v>1.029309654760062</v>
       </c>
       <c r="G11" t="n">
-        <v>1.0178142786026</v>
+        <v>1.025332808494568</v>
       </c>
     </row>
     <row r="12">
@@ -1929,7 +1929,7 @@
         <v>1.030148952032964</v>
       </c>
       <c r="G12" t="n">
-        <v>1.020101547241211</v>
+        <v>1.024316906929016</v>
       </c>
     </row>
     <row r="13">
@@ -1956,7 +1956,7 @@
         <v>1.030116034335134</v>
       </c>
       <c r="G13" t="n">
-        <v>1.013195276260376</v>
+        <v>1.020912289619446</v>
       </c>
     </row>
     <row r="14">
@@ -1983,7 +1983,7 @@
         <v>1.045967376262004</v>
       </c>
       <c r="G14" t="n">
-        <v>1.02520227432251</v>
+        <v>1.02463972568512</v>
       </c>
     </row>
     <row r="15">
@@ -2010,7 +2010,7 @@
         <v>1.046635874317729</v>
       </c>
       <c r="G15" t="n">
-        <v>1.018222570419312</v>
+        <v>1.029813289642334</v>
       </c>
     </row>
     <row r="16">
@@ -2037,7 +2037,7 @@
         <v>1.024974637370608</v>
       </c>
       <c r="G16" t="n">
-        <v>1.018589735031128</v>
+        <v>1.02247416973114</v>
       </c>
     </row>
     <row r="17">
@@ -2064,7 +2064,7 @@
         <v>1.024898383417263</v>
       </c>
       <c r="G17" t="n">
-        <v>1.015405178070068</v>
+        <v>1.023364901542664</v>
       </c>
     </row>
     <row r="18">
@@ -2091,7 +2091,7 @@
         <v>1.024856189892978</v>
       </c>
       <c r="G18" t="n">
-        <v>1.020787596702576</v>
+        <v>1.023979306221008</v>
       </c>
     </row>
     <row r="19">
@@ -2118,7 +2118,7 @@
         <v>1.024823181204229</v>
       </c>
       <c r="G19" t="n">
-        <v>1.016081213951111</v>
+        <v>1.027941703796387</v>
       </c>
     </row>
     <row r="20">
@@ -2853,7 +2853,7 @@
         <v>1.010048281792376</v>
       </c>
       <c r="G2" t="n">
-        <v>1.007017135620117</v>
+        <v>1.020681381225586</v>
       </c>
     </row>
     <row r="3">
@@ -2880,7 +2880,7 @@
         <v>1.016883932948234</v>
       </c>
       <c r="G3" t="n">
-        <v>1.017449498176575</v>
+        <v>1.022453546524048</v>
       </c>
     </row>
     <row r="4">
@@ -2907,7 +2907,7 @@
         <v>1.023729595741203</v>
       </c>
       <c r="G4" t="n">
-        <v>1.01718282699585</v>
+        <v>1.020331621170044</v>
       </c>
     </row>
     <row r="5">
@@ -2934,7 +2934,7 @@
         <v>1.023777196296011</v>
       </c>
       <c r="G5" t="n">
-        <v>1.007306337356567</v>
+        <v>1.028133273124695</v>
       </c>
     </row>
     <row r="6">
@@ -2961,7 +2961,7 @@
         <v>1.026439837996932</v>
       </c>
       <c r="G6" t="n">
-        <v>1.020736455917358</v>
+        <v>1.029252529144287</v>
       </c>
     </row>
     <row r="7">
@@ -2988,7 +2988,7 @@
         <v>1.026614266709089</v>
       </c>
       <c r="G7" t="n">
-        <v>1.014546036720276</v>
+        <v>1.023064136505127</v>
       </c>
     </row>
     <row r="8">
@@ -3015,7 +3015,7 @@
         <v>1.026867079335489</v>
       </c>
       <c r="G8" t="n">
-        <v>1.013060688972473</v>
+        <v>1.023321270942688</v>
       </c>
     </row>
     <row r="9">
@@ -3042,7 +3042,7 @@
         <v>1.027173931631028</v>
       </c>
       <c r="G9" t="n">
-        <v>1.013654112815857</v>
+        <v>1.025023102760315</v>
       </c>
     </row>
     <row r="10">
@@ -3069,7 +3069,7 @@
         <v>1.027904381417253</v>
       </c>
       <c r="G10" t="n">
-        <v>1.009623765945435</v>
+        <v>1.02395486831665</v>
       </c>
     </row>
     <row r="11">
@@ -3096,7 +3096,7 @@
         <v>1.027940725101416</v>
       </c>
       <c r="G11" t="n">
-        <v>1.016516923904419</v>
+        <v>1.024209260940552</v>
       </c>
     </row>
     <row r="12">
@@ -3123,7 +3123,7 @@
         <v>1.028785079546287</v>
       </c>
       <c r="G12" t="n">
-        <v>1.018863916397095</v>
+        <v>1.022901773452759</v>
       </c>
     </row>
     <row r="13">
@@ -3150,7 +3150,7 @@
         <v>1.02875185786923</v>
       </c>
       <c r="G13" t="n">
-        <v>1.012078404426575</v>
+        <v>1.019897222518921</v>
       </c>
     </row>
     <row r="14">
@@ -3177,7 +3177,7 @@
         <v>1.044707242702215</v>
       </c>
       <c r="G14" t="n">
-        <v>1.023532748222351</v>
+        <v>1.02352774143219</v>
       </c>
     </row>
     <row r="15">
@@ -3204,7 +3204,7 @@
         <v>1.045379618940963</v>
       </c>
       <c r="G15" t="n">
-        <v>1.017264246940613</v>
+        <v>1.028404712677002</v>
       </c>
     </row>
     <row r="16">
@@ -3231,7 +3231,7 @@
         <v>1.023603556850307</v>
       </c>
       <c r="G16" t="n">
-        <v>1.017600655555725</v>
+        <v>1.021548628807068</v>
       </c>
     </row>
     <row r="17">
@@ -3258,7 +3258,7 @@
         <v>1.023527469512051</v>
       </c>
       <c r="G17" t="n">
-        <v>1.014076113700867</v>
+        <v>1.022204279899597</v>
       </c>
     </row>
     <row r="18">
@@ -3285,7 +3285,7 @@
         <v>1.023485750796639</v>
       </c>
       <c r="G18" t="n">
-        <v>1.019089698791504</v>
+        <v>1.0229572057724</v>
       </c>
     </row>
     <row r="19">
@@ -3312,7 +3312,7 @@
         <v>1.023452266009556</v>
       </c>
       <c r="G19" t="n">
-        <v>1.014946818351746</v>
+        <v>1.026838898658752</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
Added AutoML (H2O, Autogluon, AutoSklearn) frameworks and reported results
</commit_message>
<xml_diff>
--- a/net18/validation_data/Scenario1.xlsx
+++ b/net18/validation_data/Scenario1.xlsx
@@ -398,7 +398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
@@ -440,6 +440,21 @@
           <t>Valori stimati MLP</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Valori stimati autogloun</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Valori stimati h2o</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Valori stimati autosklearn</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -465,7 +480,16 @@
         <v>1.009610254607564</v>
       </c>
       <c r="G2" t="n">
-        <v>1.01953387260437</v>
+        <v>1.027590274810791</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.019942760467529</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.020192623774532</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.020403351634741</v>
       </c>
     </row>
     <row r="3">
@@ -492,7 +516,16 @@
         <v>1.016476486950764</v>
       </c>
       <c r="G3" t="n">
-        <v>1.02214777469635</v>
+        <v>1.025810599327087</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.021311640739441</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.020923241330554</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.021254988387227</v>
       </c>
     </row>
     <row r="4">
@@ -519,7 +552,16 @@
         <v>1.023316741954023</v>
       </c>
       <c r="G4" t="n">
-        <v>1.019710302352905</v>
+        <v>1.025840163230896</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.022302865982056</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1.021639801118448</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.022154152393341</v>
       </c>
     </row>
     <row r="5">
@@ -546,7 +588,16 @@
         <v>1.023364330000336</v>
       </c>
       <c r="G5" t="n">
-        <v>1.026696681976318</v>
+        <v>1.025842189788818</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.022504806518555</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.021672062462499</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.022143915295601</v>
       </c>
     </row>
     <row r="6">
@@ -573,7 +624,16 @@
         <v>1.026025634011175</v>
       </c>
       <c r="G6" t="n">
-        <v>1.029133081436157</v>
+        <v>1.026240468025208</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.023157715797424</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.02192421087299</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.022460140287876</v>
       </c>
     </row>
     <row r="7">
@@ -600,7 +660,16 @@
         <v>1.026199926318352</v>
       </c>
       <c r="G7" t="n">
-        <v>1.02318811416626</v>
+        <v>1.026274681091309</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.023244023323059</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.021933241163622</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.022542841732502</v>
       </c>
     </row>
     <row r="8">
@@ -627,7 +696,16 @@
         <v>1.026453977738033</v>
       </c>
       <c r="G8" t="n">
-        <v>1.022620916366577</v>
+        <v>1.026357293128967</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.023131251335144</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.021974255805259</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.022584833204746</v>
       </c>
     </row>
     <row r="9">
@@ -654,7 +732,16 @@
         <v>1.026757375641291</v>
       </c>
       <c r="G9" t="n">
-        <v>1.02508008480072</v>
+        <v>1.026337862014771</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.023283123970032</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.021988076388508</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.022589188069105</v>
       </c>
     </row>
     <row r="10">
@@ -681,7 +768,16 @@
         <v>1.027484927913494</v>
       </c>
       <c r="G10" t="n">
-        <v>1.023085594177246</v>
+        <v>1.02642035484314</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.023334503173828</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.022066524096482</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.022666376084089</v>
       </c>
     </row>
     <row r="11">
@@ -708,7 +804,16 @@
         <v>1.02752103198984</v>
       </c>
       <c r="G11" t="n">
-        <v>1.02351188659668</v>
+        <v>1.02642834186554</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.023093223571777</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.02208223828959</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.02283438667655</v>
       </c>
     </row>
     <row r="12">
@@ -735,7 +840,16 @@
         <v>1.028363406436452</v>
       </c>
       <c r="G12" t="n">
-        <v>1.022902965545654</v>
+        <v>1.02669370174408</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.023193836212158</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.022137369174121</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1.022767337039113</v>
       </c>
     </row>
     <row r="13">
@@ -762,7 +876,16 @@
         <v>1.0283301717721</v>
       </c>
       <c r="G13" t="n">
-        <v>1.019252777099609</v>
+        <v>1.02667248249054</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.023270845413208</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.022149941661986</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.022821225225925</v>
       </c>
     </row>
     <row r="14">
@@ -789,7 +912,16 @@
         <v>1.044251762033414</v>
       </c>
       <c r="G14" t="n">
-        <v>1.023057222366333</v>
+        <v>1.032123923301697</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.025158047676086</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.023700070941563</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1.024323923513293</v>
       </c>
     </row>
     <row r="15">
@@ -816,7 +948,16 @@
         <v>1.04492271942274</v>
       </c>
       <c r="G15" t="n">
-        <v>1.027686476707458</v>
+        <v>1.032360434532166</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.025078058242798</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1.023769287912502</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1.024388624355197</v>
       </c>
     </row>
     <row r="16">
@@ -843,7 +984,16 @@
         <v>1.023190609422364</v>
       </c>
       <c r="G16" t="n">
-        <v>1.020583033561707</v>
+        <v>1.025725960731506</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.022520303726196</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1.021640980568508</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1.02209953777492</v>
       </c>
     </row>
     <row r="17">
@@ -870,7 +1020,16 @@
         <v>1.023114485772568</v>
       </c>
       <c r="G17" t="n">
-        <v>1.022072911262512</v>
+        <v>1.025674939155579</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.022416830062866</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1.021639523861721</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1.022209756076336</v>
       </c>
     </row>
     <row r="18">
@@ -897,7 +1056,16 @@
         <v>1.023072713401121</v>
       </c>
       <c r="G18" t="n">
-        <v>1.022224307060242</v>
+        <v>1.025647401809692</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.022548317909241</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.021637508723574</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1.022130791097879</v>
       </c>
     </row>
     <row r="19">
@@ -924,7 +1092,16 @@
         <v>1.023039265031769</v>
       </c>
       <c r="G19" t="n">
-        <v>1.026463747024536</v>
+        <v>1.025624513626099</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1.022569298744202</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1.021622429577075</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1.022023737430573</v>
       </c>
     </row>
     <row r="20">
@@ -1591,7 +1768,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
@@ -1634,6 +1811,21 @@
           <t>Valori stimati MLP</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Valori stimati autogloun</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Valori stimati h2o</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Valori stimati autosklearn</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1659,7 +1851,16 @@
         <v>1.011403376800376</v>
       </c>
       <c r="G2" t="n">
-        <v>1.021594643592834</v>
+        <v>1.029593706130981</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.021716117858887</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.021859761950581</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.022270161658525</v>
       </c>
     </row>
     <row r="3">
@@ -1686,7 +1887,16 @@
         <v>1.018252058687226</v>
       </c>
       <c r="G3" t="n">
-        <v>1.023833155632019</v>
+        <v>1.028064727783203</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.023112297058105</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.022616147704591</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.023100392892957</v>
       </c>
     </row>
     <row r="4">
@@ -1713,7 +1923,16 @@
         <v>1.025101075990773</v>
       </c>
       <c r="G4" t="n">
-        <v>1.021430492401123</v>
+        <v>1.028113484382629</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.024274230003357</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1.023330375588826</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.023942733183503</v>
       </c>
     </row>
     <row r="5">
@@ -1740,7 +1959,16 @@
         <v>1.02514865054941</v>
       </c>
       <c r="G5" t="n">
-        <v>1.028966069221497</v>
+        <v>1.028115749359131</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.024326920509338</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.023364182288714</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.023984387516975</v>
       </c>
     </row>
     <row r="6">
@@ -1767,7 +1995,16 @@
         <v>1.027809866721116</v>
       </c>
       <c r="G6" t="n">
-        <v>1.030413389205933</v>
+        <v>1.028516530990601</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.025005221366882</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.023614515168698</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.024216698482633</v>
       </c>
     </row>
     <row r="7">
@@ -1794,7 +2031,16 @@
         <v>1.027984181911415</v>
       </c>
       <c r="G7" t="n">
-        <v>1.024636745452881</v>
+        <v>1.028550982475281</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.024971604347229</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.023622743192304</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.024308227002621</v>
       </c>
     </row>
     <row r="8">
@@ -1821,7 +2067,16 @@
         <v>1.028237317852879</v>
       </c>
       <c r="G8" t="n">
-        <v>1.024176955223083</v>
+        <v>1.028632879257202</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.024969816207886</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.023662649086124</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.024393614381552</v>
       </c>
     </row>
     <row r="9">
@@ -1848,7 +2103,16 @@
         <v>1.028543542261516</v>
       </c>
       <c r="G9" t="n">
-        <v>1.026232361793518</v>
+        <v>1.028615355491638</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.025191903114319</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.023677071303612</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.024362998083234</v>
       </c>
     </row>
     <row r="10">
@@ -1875,7 +2139,16 @@
         <v>1.029273545776454</v>
       </c>
       <c r="G10" t="n">
-        <v>1.024853467941284</v>
+        <v>1.028699636459351</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.025081276893616</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.023758743405119</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.024445202201605</v>
       </c>
     </row>
     <row r="11">
@@ -1902,7 +2175,16 @@
         <v>1.029309654760062</v>
       </c>
       <c r="G11" t="n">
-        <v>1.025332808494568</v>
+        <v>1.02870762348175</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.024889588356018</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.023773435578957</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.024532794952393</v>
       </c>
     </row>
     <row r="12">
@@ -1929,7 +2211,16 @@
         <v>1.030148952032964</v>
       </c>
       <c r="G12" t="n">
-        <v>1.024316906929016</v>
+        <v>1.028972625732422</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.024939060211182</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.0238265034959</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1.024550132453442</v>
       </c>
     </row>
     <row r="13">
@@ -1956,7 +2247,16 @@
         <v>1.030116034335134</v>
       </c>
       <c r="G13" t="n">
-        <v>1.020912289619446</v>
+        <v>1.028951525688171</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.025027394294739</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.023837885363732</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.024615235626698</v>
       </c>
     </row>
     <row r="14">
@@ -1983,7 +2283,16 @@
         <v>1.045967376262004</v>
       </c>
       <c r="G14" t="n">
-        <v>1.02463972568512</v>
+        <v>1.034380435943604</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.026807904243469</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.025371825666343</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1.025975652039051</v>
       </c>
     </row>
     <row r="15">
@@ -2010,7 +2319,16 @@
         <v>1.046635874317729</v>
       </c>
       <c r="G15" t="n">
-        <v>1.029813289642334</v>
+        <v>1.034617304801941</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.026871919631958</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1.025440093339086</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1.026066292077303</v>
       </c>
     </row>
     <row r="16">
@@ -2037,7 +2355,16 @@
         <v>1.024974637370608</v>
       </c>
       <c r="G16" t="n">
-        <v>1.02247416973114</v>
+        <v>1.028000712394714</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.024463653564453</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1.023332421304764</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1.023930778726935</v>
       </c>
     </row>
     <row r="17">
@@ -2064,7 +2391,16 @@
         <v>1.024898383417263</v>
       </c>
       <c r="G17" t="n">
-        <v>1.023364901542664</v>
+        <v>1.027950167655945</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.024410486221313</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1.023331941790739</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1.023992216214538</v>
       </c>
     </row>
     <row r="18">
@@ -2091,7 +2427,16 @@
         <v>1.024856189892978</v>
       </c>
       <c r="G18" t="n">
-        <v>1.023979306221008</v>
+        <v>1.027922868728638</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.024537563323975</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.023328702466601</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1.023992385715246</v>
       </c>
     </row>
     <row r="19">
@@ -2118,7 +2463,16 @@
         <v>1.024823181204229</v>
       </c>
       <c r="G19" t="n">
-        <v>1.027941703796387</v>
+        <v>1.027900218963623</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1.024486184120178</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1.023315533862272</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1.023907117545605</v>
       </c>
     </row>
     <row r="20">
@@ -2785,7 +3139,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
@@ -2828,6 +3182,21 @@
           <t>Valori stimati MLP</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Valori stimati autogloun</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Valori stimati h2o</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Valori stimati autosklearn</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -2853,7 +3222,16 @@
         <v>1.010048281792376</v>
       </c>
       <c r="G2" t="n">
-        <v>1.020681381225586</v>
+        <v>1.028146266937256</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.020262360572815</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.020357067382873</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1.020799193531275</v>
       </c>
     </row>
     <row r="3">
@@ -2880,7 +3258,16 @@
         <v>1.016883932948234</v>
       </c>
       <c r="G3" t="n">
-        <v>1.022453546524048</v>
+        <v>1.026573419570923</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.021763682365417</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.021121925789466</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.021679824218154</v>
       </c>
     </row>
     <row r="4">
@@ -2907,7 +3294,16 @@
         <v>1.023729595741203</v>
       </c>
       <c r="G4" t="n">
-        <v>1.020331621170044</v>
+        <v>1.026589870452881</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.02286171913147</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1.021840670341476</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1.022544465959072</v>
       </c>
     </row>
     <row r="5">
@@ -2934,7 +3330,16 @@
         <v>1.023777196296011</v>
       </c>
       <c r="G5" t="n">
-        <v>1.028133273124695</v>
+        <v>1.026592016220093</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.022934675216675</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.021873419395756</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.022502392530441</v>
       </c>
     </row>
     <row r="6">
@@ -2961,7 +3366,16 @@
         <v>1.026439837996932</v>
       </c>
       <c r="G6" t="n">
-        <v>1.029252529144287</v>
+        <v>1.026983380317688</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.023601055145264</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.022126654256739</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1.02282833494246</v>
       </c>
     </row>
     <row r="7">
@@ -2988,7 +3402,16 @@
         <v>1.026614266709089</v>
       </c>
       <c r="G7" t="n">
-        <v>1.023064136505127</v>
+        <v>1.02701723575592</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.023615479469299</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.022136641153559</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.022885486483574</v>
       </c>
     </row>
     <row r="8">
@@ -3015,7 +3438,16 @@
         <v>1.026867079335489</v>
       </c>
       <c r="G8" t="n">
-        <v>1.023321270942688</v>
+        <v>1.027099370956421</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.02363395690918</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.022175798400352</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1.022984454408288</v>
       </c>
     </row>
     <row r="9">
@@ -3042,7 +3474,16 @@
         <v>1.027173931631028</v>
       </c>
       <c r="G9" t="n">
-        <v>1.025023102760315</v>
+        <v>1.02707827091217</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.023738980293274</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.02218923435227</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.022941535338759</v>
       </c>
     </row>
     <row r="10">
@@ -3069,7 +3510,16 @@
         <v>1.027904381417253</v>
       </c>
       <c r="G10" t="n">
-        <v>1.02395486831665</v>
+        <v>1.027158260345459</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.023633360862732</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1.022272775235017</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.023027962073684</v>
       </c>
     </row>
     <row r="11">
@@ -3096,7 +3546,16 @@
         <v>1.027940725101416</v>
       </c>
       <c r="G11" t="n">
-        <v>1.024209260940552</v>
+        <v>1.027166128158569</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.023514747619629</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.022286631946801</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.023161510005593</v>
       </c>
     </row>
     <row r="12">
@@ -3123,7 +3582,16 @@
         <v>1.028785079546287</v>
       </c>
       <c r="G12" t="n">
-        <v>1.022901773452759</v>
+        <v>1.02742862701416</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.023550868034363</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.022340717738838</v>
+      </c>
+      <c r="J12" t="n">
+        <v>1.023122208192945</v>
       </c>
     </row>
     <row r="13">
@@ -3150,7 +3618,16 @@
         <v>1.02875185786923</v>
       </c>
       <c r="G13" t="n">
-        <v>1.019897222518921</v>
+        <v>1.02740752696991</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.023656129837036</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.022351701328981</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.023185610771179</v>
       </c>
     </row>
     <row r="14">
@@ -3177,7 +3654,16 @@
         <v>1.044707242702215</v>
       </c>
       <c r="G14" t="n">
-        <v>1.02352774143219</v>
+        <v>1.032793641090393</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.025444984436035</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.023910220429243</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1.024646738544106</v>
       </c>
     </row>
     <row r="15">
@@ -3204,7 +3690,16 @@
         <v>1.045379618940963</v>
       </c>
       <c r="G15" t="n">
-        <v>1.028404712677002</v>
+        <v>1.033028841018677</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1.025494456291199</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1.023981344830107</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1.024717016145587</v>
       </c>
     </row>
     <row r="16">
@@ -3231,7 +3726,16 @@
         <v>1.023603556850307</v>
       </c>
       <c r="G16" t="n">
-        <v>1.021548628807068</v>
+        <v>1.026476860046387</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.023042798042297</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1.021843167464445</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1.022486876696348</v>
       </c>
     </row>
     <row r="17">
@@ -3258,7 +3762,16 @@
         <v>1.023527469512051</v>
       </c>
       <c r="G17" t="n">
-        <v>1.022204279899597</v>
+        <v>1.026426315307617</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.022890329360962</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1.02184105456308</v>
+      </c>
+      <c r="J17" t="n">
+        <v>1.022565955296159</v>
       </c>
     </row>
     <row r="18">
@@ -3285,7 +3798,16 @@
         <v>1.023485750796639</v>
       </c>
       <c r="G18" t="n">
-        <v>1.0229572057724</v>
+        <v>1.0263991355896</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.022961139678955</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.021837542433886</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1.022543009370565</v>
       </c>
     </row>
     <row r="19">
@@ -3312,7 +3834,16 @@
         <v>1.023452266009556</v>
       </c>
       <c r="G19" t="n">
-        <v>1.026838898658752</v>
+        <v>1.026376247406006</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1.022940039634705</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1.021827112642556</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1.022475566715002</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
nni for mlp fix (and updated mlp parameters in scripts)
</commit_message>
<xml_diff>
--- a/net18/validation_data/Scenario1.xlsx
+++ b/net18/validation_data/Scenario1.xlsx
@@ -480,7 +480,7 @@
         <v>1.009610254607564</v>
       </c>
       <c r="G2" t="n">
-        <v>1.027590274810791</v>
+        <v>1.022779941558838</v>
       </c>
       <c r="H2" t="n">
         <v>1.019942760467529</v>
@@ -516,7 +516,7 @@
         <v>1.016476486950764</v>
       </c>
       <c r="G3" t="n">
-        <v>1.025810599327087</v>
+        <v>1.024462223052979</v>
       </c>
       <c r="H3" t="n">
         <v>1.021311640739441</v>
@@ -552,7 +552,7 @@
         <v>1.023316741954023</v>
       </c>
       <c r="G4" t="n">
-        <v>1.025840163230896</v>
+        <v>1.025253653526306</v>
       </c>
       <c r="H4" t="n">
         <v>1.022302865982056</v>
@@ -588,7 +588,7 @@
         <v>1.023364330000336</v>
       </c>
       <c r="G5" t="n">
-        <v>1.025842189788818</v>
+        <v>1.025259852409363</v>
       </c>
       <c r="H5" t="n">
         <v>1.022504806518555</v>
@@ -624,7 +624,7 @@
         <v>1.026025634011175</v>
       </c>
       <c r="G6" t="n">
-        <v>1.026240468025208</v>
+        <v>1.025614857673645</v>
       </c>
       <c r="H6" t="n">
         <v>1.023157715797424</v>
@@ -660,7 +660,7 @@
         <v>1.026199926318352</v>
       </c>
       <c r="G7" t="n">
-        <v>1.026274681091309</v>
+        <v>1.025639653205872</v>
       </c>
       <c r="H7" t="n">
         <v>1.023244023323059</v>
@@ -696,7 +696,7 @@
         <v>1.026453977738033</v>
       </c>
       <c r="G8" t="n">
-        <v>1.026357293128967</v>
+        <v>1.025715231895447</v>
       </c>
       <c r="H8" t="n">
         <v>1.023131251335144</v>
@@ -732,7 +732,7 @@
         <v>1.026757375641291</v>
       </c>
       <c r="G9" t="n">
-        <v>1.026337862014771</v>
+        <v>1.025654435157776</v>
       </c>
       <c r="H9" t="n">
         <v>1.023283123970032</v>
@@ -768,7 +768,7 @@
         <v>1.027484927913494</v>
       </c>
       <c r="G10" t="n">
-        <v>1.02642035484314</v>
+        <v>1.025674819946289</v>
       </c>
       <c r="H10" t="n">
         <v>1.023334503173828</v>
@@ -804,7 +804,7 @@
         <v>1.02752103198984</v>
       </c>
       <c r="G11" t="n">
-        <v>1.02642834186554</v>
+        <v>1.025676608085632</v>
       </c>
       <c r="H11" t="n">
         <v>1.023093223571777</v>
@@ -840,7 +840,7 @@
         <v>1.028363406436452</v>
       </c>
       <c r="G12" t="n">
-        <v>1.02669370174408</v>
+        <v>1.025761842727661</v>
       </c>
       <c r="H12" t="n">
         <v>1.023193836212158</v>
@@ -876,7 +876,7 @@
         <v>1.0283301717721</v>
       </c>
       <c r="G13" t="n">
-        <v>1.02667248249054</v>
+        <v>1.025752544403076</v>
       </c>
       <c r="H13" t="n">
         <v>1.023270845413208</v>
@@ -912,7 +912,7 @@
         <v>1.044251762033414</v>
       </c>
       <c r="G14" t="n">
-        <v>1.032123923301697</v>
+        <v>1.027521014213562</v>
       </c>
       <c r="H14" t="n">
         <v>1.025158047676086</v>
@@ -948,7 +948,7 @@
         <v>1.04492271942274</v>
       </c>
       <c r="G15" t="n">
-        <v>1.032360434532166</v>
+        <v>1.027605056762695</v>
       </c>
       <c r="H15" t="n">
         <v>1.025078058242798</v>
@@ -984,7 +984,7 @@
         <v>1.023190609422364</v>
       </c>
       <c r="G16" t="n">
-        <v>1.025725960731506</v>
+        <v>1.025223135948181</v>
       </c>
       <c r="H16" t="n">
         <v>1.022520303726196</v>
@@ -1020,7 +1020,7 @@
         <v>1.023114485772568</v>
       </c>
       <c r="G17" t="n">
-        <v>1.025674939155579</v>
+        <v>1.025207042694092</v>
       </c>
       <c r="H17" t="n">
         <v>1.022416830062866</v>
@@ -1056,7 +1056,7 @@
         <v>1.023072713401121</v>
       </c>
       <c r="G18" t="n">
-        <v>1.025647401809692</v>
+        <v>1.025197982788086</v>
       </c>
       <c r="H18" t="n">
         <v>1.022548317909241</v>
@@ -1092,7 +1092,7 @@
         <v>1.023039265031769</v>
       </c>
       <c r="G19" t="n">
-        <v>1.025624513626099</v>
+        <v>1.025191307067871</v>
       </c>
       <c r="H19" t="n">
         <v>1.022569298744202</v>
@@ -1851,7 +1851,7 @@
         <v>1.011403376800376</v>
       </c>
       <c r="G2" t="n">
-        <v>1.029593706130981</v>
+        <v>1.024691820144653</v>
       </c>
       <c r="H2" t="n">
         <v>1.021716117858887</v>
@@ -1887,7 +1887,7 @@
         <v>1.018252058687226</v>
       </c>
       <c r="G3" t="n">
-        <v>1.028064727783203</v>
+        <v>1.026421546936035</v>
       </c>
       <c r="H3" t="n">
         <v>1.023112297058105</v>
@@ -1923,7 +1923,7 @@
         <v>1.025101075990773</v>
       </c>
       <c r="G4" t="n">
-        <v>1.028113484382629</v>
+        <v>1.027212977409363</v>
       </c>
       <c r="H4" t="n">
         <v>1.024274230003357</v>
@@ -1959,7 +1959,7 @@
         <v>1.02514865054941</v>
       </c>
       <c r="G5" t="n">
-        <v>1.028115749359131</v>
+        <v>1.02721905708313</v>
       </c>
       <c r="H5" t="n">
         <v>1.024326920509338</v>
@@ -1995,7 +1995,7 @@
         <v>1.027809866721116</v>
       </c>
       <c r="G6" t="n">
-        <v>1.028516530990601</v>
+        <v>1.027571320533752</v>
       </c>
       <c r="H6" t="n">
         <v>1.025005221366882</v>
@@ -2031,7 +2031,7 @@
         <v>1.027984181911415</v>
       </c>
       <c r="G7" t="n">
-        <v>1.028550982475281</v>
+        <v>1.0275958776474</v>
       </c>
       <c r="H7" t="n">
         <v>1.024971604347229</v>
@@ -2067,7 +2067,7 @@
         <v>1.028237317852879</v>
       </c>
       <c r="G8" t="n">
-        <v>1.028632879257202</v>
+        <v>1.027671575546265</v>
       </c>
       <c r="H8" t="n">
         <v>1.024969816207886</v>
@@ -2103,7 +2103,7 @@
         <v>1.028543542261516</v>
       </c>
       <c r="G9" t="n">
-        <v>1.028615355491638</v>
+        <v>1.027608513832092</v>
       </c>
       <c r="H9" t="n">
         <v>1.025191903114319</v>
@@ -2139,7 +2139,7 @@
         <v>1.029273545776454</v>
       </c>
       <c r="G10" t="n">
-        <v>1.028699636459351</v>
+        <v>1.027626276016235</v>
       </c>
       <c r="H10" t="n">
         <v>1.025081276893616</v>
@@ -2175,7 +2175,7 @@
         <v>1.029309654760062</v>
       </c>
       <c r="G11" t="n">
-        <v>1.02870762348175</v>
+        <v>1.027627825737</v>
       </c>
       <c r="H11" t="n">
         <v>1.024889588356018</v>
@@ -2211,7 +2211,7 @@
         <v>1.030148952032964</v>
       </c>
       <c r="G12" t="n">
-        <v>1.028972625732422</v>
+        <v>1.027709603309631</v>
       </c>
       <c r="H12" t="n">
         <v>1.024939060211182</v>
@@ -2247,7 +2247,7 @@
         <v>1.030116034335134</v>
       </c>
       <c r="G13" t="n">
-        <v>1.028951525688171</v>
+        <v>1.027700543403625</v>
       </c>
       <c r="H13" t="n">
         <v>1.025027394294739</v>
@@ -2283,7 +2283,7 @@
         <v>1.045967376262004</v>
       </c>
       <c r="G14" t="n">
-        <v>1.034380435943604</v>
+        <v>1.029393672943115</v>
       </c>
       <c r="H14" t="n">
         <v>1.026807904243469</v>
@@ -2319,7 +2319,7 @@
         <v>1.046635874317729</v>
       </c>
       <c r="G15" t="n">
-        <v>1.034617304801941</v>
+        <v>1.029475450515747</v>
       </c>
       <c r="H15" t="n">
         <v>1.026871919631958</v>
@@ -2355,7 +2355,7 @@
         <v>1.024974637370608</v>
       </c>
       <c r="G16" t="n">
-        <v>1.028000712394714</v>
+        <v>1.027183532714844</v>
       </c>
       <c r="H16" t="n">
         <v>1.024463653564453</v>
@@ -2391,7 +2391,7 @@
         <v>1.024898383417263</v>
       </c>
       <c r="G17" t="n">
-        <v>1.027950167655945</v>
+        <v>1.027167916297913</v>
       </c>
       <c r="H17" t="n">
         <v>1.024410486221313</v>
@@ -2427,7 +2427,7 @@
         <v>1.024856189892978</v>
       </c>
       <c r="G18" t="n">
-        <v>1.027922868728638</v>
+        <v>1.027159214019775</v>
       </c>
       <c r="H18" t="n">
         <v>1.024537563323975</v>
@@ -2463,7 +2463,7 @@
         <v>1.024823181204229</v>
       </c>
       <c r="G19" t="n">
-        <v>1.027900218963623</v>
+        <v>1.027152538299561</v>
       </c>
       <c r="H19" t="n">
         <v>1.024486184120178</v>
@@ -3222,7 +3222,7 @@
         <v>1.010048281792376</v>
       </c>
       <c r="G2" t="n">
-        <v>1.028146266937256</v>
+        <v>1.023244738578796</v>
       </c>
       <c r="H2" t="n">
         <v>1.020262360572815</v>
@@ -3258,7 +3258,7 @@
         <v>1.016883932948234</v>
       </c>
       <c r="G3" t="n">
-        <v>1.026573419570923</v>
+        <v>1.024979948997498</v>
       </c>
       <c r="H3" t="n">
         <v>1.021763682365417</v>
@@ -3294,7 +3294,7 @@
         <v>1.023729595741203</v>
       </c>
       <c r="G4" t="n">
-        <v>1.026589870452881</v>
+        <v>1.025766611099243</v>
       </c>
       <c r="H4" t="n">
         <v>1.02286171913147</v>
@@ -3330,7 +3330,7 @@
         <v>1.023777196296011</v>
       </c>
       <c r="G5" t="n">
-        <v>1.026592016220093</v>
+        <v>1.0257728099823</v>
       </c>
       <c r="H5" t="n">
         <v>1.022934675216675</v>
@@ -3366,7 +3366,7 @@
         <v>1.026439837996932</v>
       </c>
       <c r="G6" t="n">
-        <v>1.026983380317688</v>
+        <v>1.026127099990845</v>
       </c>
       <c r="H6" t="n">
         <v>1.023601055145264</v>
@@ -3402,7 +3402,7 @@
         <v>1.026614266709089</v>
       </c>
       <c r="G7" t="n">
-        <v>1.02701723575592</v>
+        <v>1.026151776313782</v>
       </c>
       <c r="H7" t="n">
         <v>1.023615479469299</v>
@@ -3438,7 +3438,7 @@
         <v>1.026867079335489</v>
       </c>
       <c r="G8" t="n">
-        <v>1.027099370956421</v>
+        <v>1.026228666305542</v>
       </c>
       <c r="H8" t="n">
         <v>1.02363395690918</v>
@@ -3474,7 +3474,7 @@
         <v>1.027173931631028</v>
       </c>
       <c r="G9" t="n">
-        <v>1.02707827091217</v>
+        <v>1.026163816452026</v>
       </c>
       <c r="H9" t="n">
         <v>1.023738980293274</v>
@@ -3510,7 +3510,7 @@
         <v>1.027904381417253</v>
       </c>
       <c r="G10" t="n">
-        <v>1.027158260345459</v>
+        <v>1.026180505752563</v>
       </c>
       <c r="H10" t="n">
         <v>1.023633360862732</v>
@@ -3546,7 +3546,7 @@
         <v>1.027940725101416</v>
       </c>
       <c r="G11" t="n">
-        <v>1.027166128158569</v>
+        <v>1.026182174682617</v>
       </c>
       <c r="H11" t="n">
         <v>1.023514747619629</v>
@@ -3582,7 +3582,7 @@
         <v>1.028785079546287</v>
       </c>
       <c r="G12" t="n">
-        <v>1.02742862701416</v>
+        <v>1.026266694068909</v>
       </c>
       <c r="H12" t="n">
         <v>1.023550868034363</v>
@@ -3618,7 +3618,7 @@
         <v>1.02875185786923</v>
       </c>
       <c r="G13" t="n">
-        <v>1.02740752696991</v>
+        <v>1.026257395744324</v>
       </c>
       <c r="H13" t="n">
         <v>1.023656129837036</v>
@@ -3654,7 +3654,7 @@
         <v>1.044707242702215</v>
       </c>
       <c r="G14" t="n">
-        <v>1.032793641090393</v>
+        <v>1.028006672859192</v>
       </c>
       <c r="H14" t="n">
         <v>1.025444984436035</v>
@@ -3690,7 +3690,7 @@
         <v>1.045379618940963</v>
       </c>
       <c r="G15" t="n">
-        <v>1.033028841018677</v>
+        <v>1.028090953826904</v>
       </c>
       <c r="H15" t="n">
         <v>1.025494456291199</v>
@@ -3726,7 +3726,7 @@
         <v>1.023603556850307</v>
       </c>
       <c r="G16" t="n">
-        <v>1.026476860046387</v>
+        <v>1.025736093521118</v>
       </c>
       <c r="H16" t="n">
         <v>1.023042798042297</v>
@@ -3762,7 +3762,7 @@
         <v>1.023527469512051</v>
       </c>
       <c r="G17" t="n">
-        <v>1.026426315307617</v>
+        <v>1.025720000267029</v>
       </c>
       <c r="H17" t="n">
         <v>1.022890329360962</v>
@@ -3798,7 +3798,7 @@
         <v>1.023485750796639</v>
       </c>
       <c r="G18" t="n">
-        <v>1.0263991355896</v>
+        <v>1.025711059570312</v>
       </c>
       <c r="H18" t="n">
         <v>1.022961139678955</v>
@@ -3834,7 +3834,7 @@
         <v>1.023452266009556</v>
       </c>
       <c r="G19" t="n">
-        <v>1.026376247406006</v>
+        <v>1.025704145431519</v>
       </c>
       <c r="H19" t="n">
         <v>1.022940039634705</v>

</xml_diff>